<commit_message>
Updates to AZ-104 and Example for AZ-104
</commit_message>
<xml_diff>
--- a/Assessments/Exam-Msft-AZ-104-Self-Assessment-Build5Nines.xlsx
+++ b/Assessments/Exam-Msft-AZ-104-Self-Assessment-Build5Nines.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayre\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\exam-assessments\Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5253FF8-0B85-438E-A5A6-446201CA0EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="53928" windowHeight="19656" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessment Overview" sheetId="3" r:id="rId1"/>
     <sheet name="Self Assessment" sheetId="5" r:id="rId2"/>
     <sheet name="Other Values" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -24,7 +25,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -35,12 +39,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Mark Ayre</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C59" authorId="0" shapeId="0">
+    <comment ref="C61" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C73" authorId="0" shapeId="0">
+    <comment ref="C90" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -79,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C79" authorId="0" shapeId="0">
+    <comment ref="C96" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -92,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C97" authorId="0" shapeId="0">
+    <comment ref="C111" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -105,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C103" authorId="0" shapeId="0">
+    <comment ref="C117" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="160">
   <si>
     <t>Microsoft Certification Self-Assessment Tool</t>
   </si>
@@ -218,9 +222,6 @@
     <t>create a custom role</t>
   </si>
   <si>
-    <t>generate shared access signature</t>
-  </si>
-  <si>
     <t>manage access keys</t>
   </si>
   <si>
@@ -239,18 +240,9 @@
     <t>deploy and configure scale sets</t>
   </si>
   <si>
-    <t>modify Azure Resource Manager (ARM) template</t>
-  </si>
-  <si>
-    <t>configure VHD template</t>
-  </si>
-  <si>
     <t>deploy from template</t>
   </si>
   <si>
-    <t>save a deployment as an ARM template</t>
-  </si>
-  <si>
     <t>add data discs</t>
   </si>
   <si>
@@ -263,15 +255,9 @@
     <t>redeploy VMs</t>
   </si>
   <si>
-    <t>create and configure VNET peering</t>
-  </si>
-  <si>
     <t>Implement and manage virtual networking</t>
   </si>
   <si>
-    <t>configure private and public IP addresses, network routes, network interface, subnets, and virtual network</t>
-  </si>
-  <si>
     <t>Configure name resolution</t>
   </si>
   <si>
@@ -293,9 +279,6 @@
     <t>configure self-service password reset</t>
   </si>
   <si>
-    <t>manage multiple directories</t>
-  </si>
-  <si>
     <t>manage user and group properties</t>
   </si>
   <si>
@@ -350,9 +333,6 @@
     <t>configure Azure AD Join</t>
   </si>
   <si>
-    <t>provide access to Azure resources by assigning roles (subscriptions, resource groups, resources (VM, disk, etc.)</t>
-  </si>
-  <si>
     <t>interpret access assignments</t>
   </si>
   <si>
@@ -362,18 +342,9 @@
     <t>configure Azure policies</t>
   </si>
   <si>
-    <t>apply tags</t>
-  </si>
-  <si>
-    <t>create and manage resource groups (move resources, remove RGs)</t>
-  </si>
-  <si>
     <t>manage subscriptions</t>
   </si>
   <si>
-    <t>configure Cost Management</t>
-  </si>
-  <si>
     <t>configure management groups</t>
   </si>
   <si>
@@ -383,12 +354,6 @@
     <t>create and configure storage accounts</t>
   </si>
   <si>
-    <t>configugre Azure AD Authentication for a storage account</t>
-  </si>
-  <si>
-    <t>Manage storage accounts</t>
-  </si>
-  <si>
     <t>export from Azure job</t>
   </si>
   <si>
@@ -398,9 +363,6 @@
     <t>copy data by using AZCopy</t>
   </si>
   <si>
-    <t>Manage data in Azure Storage</t>
-  </si>
-  <si>
     <t>Configure Azure files and Azure blob storage</t>
   </si>
   <si>
@@ -413,21 +375,6 @@
     <t>configure Azure blob storage</t>
   </si>
   <si>
-    <t>configure storage tiers for Azure blobs</t>
-  </si>
-  <si>
-    <t>Configure VMs for high availability and scability</t>
-  </si>
-  <si>
-    <t>Automate deployment and configuration of VMs</t>
-  </si>
-  <si>
-    <t>automate configuration management by using custom script extensions</t>
-  </si>
-  <si>
-    <t>Create and configure VMs</t>
-  </si>
-  <si>
     <t>configure Azure Disk Encryption</t>
   </si>
   <si>
@@ -437,57 +384,30 @@
     <t>create and configure Azure Kubernetes Service (AKS)</t>
   </si>
   <si>
-    <t>create and configure Azure Containers Instances (ACI)</t>
-  </si>
-  <si>
     <t>Create and configure containers</t>
   </si>
   <si>
-    <t>Create and configure Web Apps</t>
-  </si>
-  <si>
     <t>create and configure App Service</t>
   </si>
   <si>
-    <t>create and configure App Service Plans</t>
-  </si>
-  <si>
     <t>configure a private or public DNS zone</t>
   </si>
   <si>
     <t>Secure access to virtual networks</t>
   </si>
   <si>
-    <t>deploy and configure Azure Firewall</t>
-  </si>
-  <si>
-    <t>deploy and configure Azure Bastion Service</t>
-  </si>
-  <si>
     <t>Configure load balancing</t>
   </si>
   <si>
     <t>configure Application Gateway</t>
   </si>
   <si>
-    <t>configure an internal load balancer</t>
-  </si>
-  <si>
-    <t>configure load balacing rules</t>
-  </si>
-  <si>
-    <t>configure a public load balancer</t>
-  </si>
-  <si>
     <t>troubleshoot load balancing</t>
   </si>
   <si>
     <t>monitor on-premises connectivity</t>
   </si>
   <si>
-    <t>use Network Performance monitor</t>
-  </si>
-  <si>
     <t>use Network Watcher</t>
   </si>
   <si>
@@ -503,12 +423,6 @@
     <t>create and configure Azure VPN Gateway</t>
   </si>
   <si>
-    <t>create and configure VPNs</t>
-  </si>
-  <si>
-    <t>configure Express Route</t>
-  </si>
-  <si>
     <t>configure Azure Virtual WAN</t>
   </si>
   <si>
@@ -533,12 +447,6 @@
     <t>Implement backup and recovery</t>
   </si>
   <si>
-    <t>perform backup and restore operations by using Azure Backup Service</t>
-  </si>
-  <si>
-    <t>create a Recovery Services Vault (use soft delete to recovery Azure VM's)</t>
-  </si>
-  <si>
     <t>perform site-to-site recovery by using Azure Site Recovery</t>
   </si>
   <si>
@@ -558,12 +466,153 @@
   </si>
   <si>
     <t>install and use Azure Storage Explorer</t>
+  </si>
+  <si>
+    <t>create administrative units</t>
+  </si>
+  <si>
+    <t>provide access to Azure resources by assigning roles at different scopes (subscriptions, resource groups, resources (VM, disk, etc.)</t>
+  </si>
+  <si>
+    <t>apply and manage tags on resources</t>
+  </si>
+  <si>
+    <t>manage resource groups (move resources, remove RGs)</t>
+  </si>
+  <si>
+    <t>manage costs</t>
+  </si>
+  <si>
+    <t>generate shared access signature (SAS) tokens</t>
+  </si>
+  <si>
+    <t>Secure Storage</t>
+  </si>
+  <si>
+    <t>Manage Storage</t>
+  </si>
+  <si>
+    <t>configure Azure AD authentication for a storage account</t>
+  </si>
+  <si>
+    <t>configure access to Azure Files</t>
+  </si>
+  <si>
+    <t>configure blob object replication</t>
+  </si>
+  <si>
+    <t>configure storage tiers</t>
+  </si>
+  <si>
+    <t>configure blob lifecycle management</t>
+  </si>
+  <si>
+    <t>Create and configure Azure App Service</t>
+  </si>
+  <si>
+    <t>configure a virtual hard disk (VHD) template</t>
+  </si>
+  <si>
+    <t>save a deployment as an Azure Resource Manager template</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> deploy virtual machine extensions</t>
+  </si>
+  <si>
+    <t>Automate deployment of virtual machines (VMs) by using Azure Resource Manager templates</t>
+  </si>
+  <si>
+    <t>modify an Azure Resource Manager template</t>
+  </si>
+  <si>
+    <t>Configure VMs</t>
+  </si>
+  <si>
+    <t>configure sizing and scaling for Azure Container Instances</t>
+  </si>
+  <si>
+    <t>configure container groups for Azure Container Instances</t>
+  </si>
+  <si>
+    <t>configure scaling for AKS</t>
+  </si>
+  <si>
+    <t>configure network connections for AKS</t>
+  </si>
+  <si>
+    <t>upgrade an AKS cluster</t>
+  </si>
+  <si>
+    <t>configure scaling settings in an App Service plan</t>
+  </si>
+  <si>
+    <t>create an App Service</t>
+  </si>
+  <si>
+    <t>secure an App Service</t>
+  </si>
+  <si>
+    <t>configure custom domain names</t>
+  </si>
+  <si>
+    <t>configure backup for an App Service</t>
+  </si>
+  <si>
+    <t>configure networking settings</t>
+  </si>
+  <si>
+    <t>configure deployment settings</t>
+  </si>
+  <si>
+    <t>create and configure Express Route</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> create and configure virtual networks, including peering</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> configure private and public IP addresses</t>
+  </si>
+  <si>
+    <t>configure user-defined network routes</t>
+  </si>
+  <si>
+    <t>implement subnets</t>
+  </si>
+  <si>
+    <t>configure endpoints on subnets</t>
+  </si>
+  <si>
+    <t>configure private endpoints</t>
+  </si>
+  <si>
+    <t>configure Azure DNS, including custom DNS settings and private or public DNS zones</t>
+  </si>
+  <si>
+    <t>implement Azure Bastion</t>
+  </si>
+  <si>
+    <t>implement Azure Firewall</t>
+  </si>
+  <si>
+    <t>configure an internal or public load balancer</t>
+  </si>
+  <si>
+    <t>configure and use Azure Monitor for Networks</t>
+  </si>
+  <si>
+    <t>create a Recovery Services Vault (use soft delete to recover Azure VM's)</t>
+  </si>
+  <si>
+    <t>perform backup and restore operations by using Azure Backup</t>
+  </si>
+  <si>
+    <t>Updated on 6/6/2021 by Michael Bender</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -741,7 +790,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -765,6 +814,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -774,7 +835,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="138">
+  <dxfs count="126">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1227,6 +1288,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1247,6 +1318,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1257,6 +1338,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1287,6 +1388,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1407,211 +1528,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2430,77 +2371,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.19921875" customWidth="1"/>
-    <col min="2" max="2" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.25" customWidth="1"/>
+    <col min="2" max="2" width="19.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="24.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>9</v>
       </c>
@@ -2508,52 +2449,52 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B16" s="8">
         <f>'Self Assessment'!D2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B17" s="8">
         <f>'Self Assessment'!D24</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B18" s="8">
-        <f>'Self Assessment'!D42</f>
+        <f>'Self Assessment'!D45</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B19" s="8">
-        <f>'Self Assessment'!D65</f>
+        <f>'Self Assessment'!D77</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B20" s="8">
-        <f>'Self Assessment'!D96</f>
+        <f>'Self Assessment'!D110</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A21" s="12" t="s">
         <v>11</v>
       </c>
@@ -2562,31 +2503,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
     </row>
-    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
@@ -2594,7 +2535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
@@ -2602,257 +2543,265 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B16:B18 B20">
-    <cfRule type="cellIs" dxfId="137" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="125" priority="9" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B18 B20">
-    <cfRule type="cellIs" dxfId="136" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="124" priority="8" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B18 B20">
-    <cfRule type="cellIs" dxfId="135" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="123" priority="7" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="cellIs" dxfId="134" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="122" priority="6" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="cellIs" dxfId="133" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="121" priority="5" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="cellIs" dxfId="132" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="120" priority="4" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="131" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="119" priority="3" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="130" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="118" priority="2" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="129" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="117" priority="1" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D28" r:id="rId1"/>
-    <hyperlink ref="D29" r:id="rId2"/>
-    <hyperlink ref="A13" r:id="rId3"/>
-    <hyperlink ref="A33" r:id="rId4"/>
-    <hyperlink ref="A37" r:id="rId5"/>
-    <hyperlink ref="B24" r:id="rId6"/>
+    <hyperlink ref="D28" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D29" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A33" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A37" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B24" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E108"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="B86" workbookViewId="0">
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.19921875" customWidth="1"/>
-    <col min="2" max="2" width="20.59765625" customWidth="1"/>
-    <col min="3" max="3" width="37.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.25" customWidth="1"/>
+    <col min="2" max="2" width="38.875" customWidth="1"/>
+    <col min="3" max="3" width="37.125" style="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="14" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="23" t="s">
         <v>25</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>70</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C2" s="24"/>
       <c r="D2" s="11">
         <f>SUM(D3:D23)/3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>72</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C3" s="25"/>
       <c r="D3" s="8">
-        <f>(IF(D4="Know Well", 1, IF(D4="Know a Little", 0.5, 0))+IF(D5="Know Well", 1, IF(D5="Know a Little", 0.5, 0))+IF(D6="Know Well", 1, IF(D6="Know a Little", 0.5, 0))+IF(D7="Know Well", 1, IF(D7="Know a Little", 0.5, 0))+IF(D8="Know Well", 1, IF(D8="Know a Little", 0.5, 0))+IF(D9="Know Well", 1, IF(D9="Know a Little", 0.5, 0))+IF(D10="Know Well", 1, IF(D10="Know a Little", 0.5, 0)))/7</f>
+        <f>(IF(D4="Know Well", 1, IF(D4="Know a Little", 0.5, 0))+IF(D6="Know Well", 1, IF(D6="Know a Little", 0.5, 0))+IF(D7="Know Well", 1, IF(D7="Know a Little", 0.5, 0))+IF(D8="Know Well", 1, IF(D8="Know a Little", 0.5, 0))+IF(D9="Know Well", 1, IF(D9="Know a Little", 0.5, 0))+IF(D10="Know Well", 1, IF(D10="Know a Little", 0.5, 0))+IF(D11="Know Well", 1, IF(D11="Know a Little", 0.5, 0)))/7</f>
         <v>0</v>
       </c>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>73</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="26" t="s">
+        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>57</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="26" t="s">
+        <v>113</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>58</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>59</v>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="26" t="s">
+        <v>51</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>60</v>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="26" t="s">
+        <v>52</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>74</v>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="26" t="s">
+        <v>53</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>55</v>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="26" t="s">
+        <v>67</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="8">
-        <f>(IF(D12="Know Well", 1, IF(D12="Know a Little", 0.5, 0))+IF(D13="Know Well", 1, IF(D13="Know a Little", 0.5, 0))+IF(D14="Know Well", 1, IF(D14="Know a Little", 0.5, 0))+IF(D15="Know Well", 1, IF(D15="Know a Little", 0.5, 0)))/4</f>
+      <c r="C12" s="25"/>
+      <c r="D12" s="8">
+        <f>(IF(D13="Know Well", 1, IF(D13="Know a Little", 0.5, 0))+IF(D14="Know Well", 1, IF(D14="Know a Little", 0.5, 0))+IF(D15="Know Well", 1, IF(D15="Know a Little", 0.5, 0)))/3</f>
         <v>0</v>
       </c>
-      <c r="E11" s="19"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
+      <c r="E12" s="19"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>75</v>
-      </c>
       <c r="D13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>76</v>
+    <row r="14" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="C14" s="26" t="s">
+        <v>114</v>
       </c>
       <c r="D14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>56</v>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="26" t="s">
+        <v>68</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D16" s="8">
         <f>(IF(D17="Know Well", 1, IF(D17="Know a Little", 0.5, 0))+IF(D18="Know Well", 1, IF(D18="Know a Little", 0.5, 0))+IF(D19="Know Well", 1, IF(D19="Know a Little", 0.5, 0))+IF(D20="Know Well", 1, IF(D20="Know a Little", 0.5, 0))+IF(D21="Know Well", 1, IF(D21="Know a Little", 0.5, 0))+IF(D22="Know Well", 1, IF(D22="Know a Little", 0.5, 0))+IF(D23="Know Well", 1, IF(D23="Know a Little", 0.5, 0)))/7</f>
@@ -2860,1367 +2809,1436 @@
       </c>
       <c r="E16" s="21"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C20" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="11">
+        <f>SUM(D25:D43)/3</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:5" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="8">
+        <f>(IF(D26="Know Well", 1, IF(D26="Know a Little", 0.5, 0))+IF(D27="Know Well", 1, IF(D27="Know a Little", 0.5, 0))+IF(D28="Know Well", 1, IF(D28="Know a Little", 0.5, 0))+IF(D29="Know Well", 1, IF(D29="Know a Little", 0.5, 0))+IF(D31="Know Well", 1, IF(D31="Know a Little", 0.5, 0))+IF(D30="Know Well", 1, IF(D30="Know a Little", 0.5, 0)))/6</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="19"/>
+    </row>
+    <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C26" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C28" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C30" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B32" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="25"/>
+      <c r="D32" s="8">
+        <f>(IF(D33="Know Well", 1, IF(D33="Know a Little", 0.5, 0))+IF(D34="Know Well", 1, IF(D34="Know a Little", 0.5, 0))+IF(D35="Know Well", 1, IF(D35="Know a Little", 0.5, 0))+IF(D37="Know Well", 1, IF(D37="Know a Little", 0.5, 0))+IF(D38="Know Well", 1, IF(D38="Know a Little", 0.5, 0))+IF(D36="Know Well", 1, IF(D36="Know a Little", 0.5, 0)))/6</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="19"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B39" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+      <c r="C39" s="25"/>
+      <c r="D39" s="8">
+        <f>(IF(D40="Know Well", 1, IF(D40="Know a Little", 0.5, 0))+IF(D41="Know Well", 1, IF(D41="Know a Little", 0.5, 0))+IF(D42="Know Well", 1, IF(D42="Know a Little", 0.5, 0))+IF(D43="Know Well", 1, IF(D43="Know a Little", 0.5, 0))+IF(D44="Know Well", 1, IF(D44="Know a Little", 0.5, 0)))/5</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="19"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="D19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
+      <c r="D41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="D21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A24" s="6" t="s">
+      <c r="D42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="11">
-        <f>SUM(D25:D41)/3</f>
+      <c r="C45" s="24"/>
+      <c r="D45" s="11">
+        <f>SUM(D46:D70)/5</f>
         <v>0</v>
       </c>
-      <c r="E24" s="20"/>
-    </row>
-    <row r="25" spans="1:5" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B25" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="8">
-        <f>(IF(D26="Know Well", 1, IF(D26="Know a Little", 0.5, 0))+IF(D27="Know Well", 1, IF(D27="Know a Little", 0.5, 0))+IF(D28="Know Well", 1, IF(D28="Know a Little", 0.5, 0))+IF(D29="Know Well", 1, IF(D29="Know a Little", 0.5, 0))+IF(D30="Know Well", 1, IF(D30="Know a Little", 0.5, 0))+IF(D31="Know Well", 1, IF(D31="Know a Little", 0.5, 0)))/6</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="19"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B32" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" s="8">
-        <f>(IF(D33="Know Well", 1, IF(D33="Know a Little", 0.5, 0))+IF(D34="Know Well", 1, IF(D34="Know a Little", 0.5, 0))+IF(D35="Know Well", 1, IF(D35="Know a Little", 0.5, 0))+IF(D36="Know Well", 1, IF(D36="Know a Little", 0.5, 0)))/4</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="19"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C35" t="s">
-        <v>144</v>
-      </c>
-      <c r="D35" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B37" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="8">
-        <f>(IF(D38="Know Well", 1, IF(D38="Know a Little", 0.5, 0))+IF(D39="Know Well", 1, IF(D39="Know a Little", 0.5, 0))+IF(D40="Know Well", 1, IF(D40="Know a Little", 0.5, 0))+IF(D41="Know Well", 1, IF(D41="Know a Little", 0.5, 0)))/4</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="19"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C38" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C39" t="s">
-        <v>94</v>
-      </c>
-      <c r="D39" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C40" t="s">
-        <v>95</v>
-      </c>
-      <c r="D40" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
-        <v>96</v>
-      </c>
-      <c r="D41" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A42" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D42" s="11">
-        <f>SUM(D43:D64)/5</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="20"/>
-    </row>
-    <row r="43" spans="1:5" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B43" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D43" s="8">
-        <f>(IF(D44="Know Well", 1, IF(D44="Know a Little", 0.5, 0))+IF(D45="Know Well", 1, IF(D45="Know a Little", 0.5, 0)))/2</f>
-        <v>0</v>
-      </c>
-      <c r="E43" s="19"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C44" t="s">
-        <v>36</v>
-      </c>
-      <c r="D44" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C45" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="E45" s="20"/>
+    </row>
+    <row r="46" spans="1:5" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B46" s="7" t="s">
-        <v>98</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C46" s="25"/>
       <c r="D46" s="8">
         <f>(IF(D47="Know Well", 1, IF(D47="Know a Little", 0.5, 0))+IF(D48="Know Well", 1, IF(D48="Know a Little", 0.5, 0))+IF(D49="Know Well", 1, IF(D49="Know a Little", 0.5, 0))+IF(D50="Know Well", 1, IF(D50="Know a Little", 0.5, 0))+IF(D51="Know Well", 1, IF(D51="Know a Little", 0.5, 0)))/5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
+    <row r="47" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C47" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C48" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C49" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C50" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C51" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B52" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="25"/>
+      <c r="D52" s="8">
+        <f>(IF(D53="Know Well", 1, IF(D53="Know a Little", 0.5, 0))+IF(D54="Know Well", 1, IF(D54="Know a Little", 0.5, 0))+IF(D55="Know Well", 1, IF(D55="Know a Little", 0.5, 0))+IF(D56="Know Well", 1, IF(D56="Know a Little", 0.5, 0))+IF(D57="Know Well", 1, IF(D57="Know a Little", 0.5, 0))+IF(D58="Know Well", 1, IF(D58="Know a Little", 0.5, 0))+IF(D59="Know Well", 1, IF(D59="Know a Little", 0.5, 0))+IF(D60="Know Well", 1, IF(D60="Know a Little", 0.5, 0)))/8</f>
+        <v>0</v>
+      </c>
+      <c r="E52" s="19"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C53" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C54" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C55" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C56" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D48" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
-        <v>40</v>
-      </c>
-      <c r="D49" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C50" t="s">
+      <c r="D56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C57" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C58" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D50" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C51" t="s">
+      <c r="D58" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C59" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C60" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B61" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="25"/>
+      <c r="D61" s="8">
+        <f>(IF(D62="Know Well", 1, IF(D62="Know a Little", 0.5, 0))+IF(D63="Know Well", 1, IF(D63="Know a Little", 0.5, 0))+IF(D64="Know Well", 1, IF(D64="Know a Little", 0.5, 0))+IF(D65="Know Well", 1, IF(D65="Know a Little", 0.5, 0))+IF(D66="Know Well", 1, IF(D66="Know a Little", 0.5, 0))+IF(D67="Know Well", 1, IF(D67="Know a Little", 0.5, 0)))/6</f>
+        <v>0</v>
+      </c>
+      <c r="E61" s="19"/>
+    </row>
+    <row r="62" spans="2:5" s="7" customFormat="1" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="C62" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="D62" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" s="19"/>
+    </row>
+    <row r="63" spans="2:5" s="7" customFormat="1" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="C63" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="D63" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="19"/>
+    </row>
+    <row r="64" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C64" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D64" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C65" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D65" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C66" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="D66" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C67" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D67" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B68" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D68" s="8">
+        <f>(IF(D69="Know Well", 1, IF(D69="Know a Little", 0.5, 0))+IF(D70="Know Well", 1, IF(D70="Know a Little", 0.5, 0))+IF(D71="Know Well", 1, IF(D71="Know a Little", 0.5, 0))+IF(D72="Know Well", 1, IF(D72="Know a Little", 0.5, 0))+IF(D73="Know Well", 1, IF(D73="Know a Little", 0.5, 0))+IF(D74="Know Well", 1, IF(D74="Know a Little", 0.5, 0))+IF(D75="Know Well", 1, IF(D75="Know a Little", 0.5, 0))+IF(D76="Know Well", 1, IF(D76="Know a Little", 0.5, 0)))/8</f>
+        <v>0</v>
+      </c>
+      <c r="E68" s="21"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C69" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C70" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="D70" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C71" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="D71" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C72" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="D72" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C73" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="D73" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C74" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="D74" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C75" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="D75" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C76" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D76" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A77" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C77" s="24"/>
+      <c r="D77" s="11">
+        <f>SUM(D78:D109)/6</f>
+        <v>0</v>
+      </c>
+      <c r="E77" s="20"/>
+    </row>
+    <row r="78" spans="1:5" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B78" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C78" s="25"/>
+      <c r="D78" s="8">
+        <f>(IF(D79="Know Well", 1, IF(D79="Know a Little", 0.5, 0))+IF(D80="Know Well", 1, IF(D80="Know a Little", 0.5, 0))+IF(D81="Know Well", 1, IF(D81="Know a Little", 0.5, 0))+IF(D82="Know Well", 1, IF(D82="Know a Little", 0.5, 0))+IF(D83="Know Well", 1, IF(D83="Know a Little", 0.5, 0))+IF(D84="Know Well", 1, IF(D84="Know a Little", 0.5, 0))+IF(D85="Know Well", 1, IF(D85="Know a Little", 0.5, 0)))/7</f>
+        <v>0</v>
+      </c>
+      <c r="E78" s="19"/>
+    </row>
+    <row r="79" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C79" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="D79" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C80" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="D80" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C81" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="D81" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C82" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D82" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C83" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D83" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C84" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D84" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C85" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D85" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B86" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C86" s="25"/>
+      <c r="D86" s="8">
+        <f>(IF(D87="Know Well", 1, IF(D87="Know a Little", 0.5, 0))+IF(D88="Know Well", 1, IF(D88="Know a Little", 0.5, 0))+IF(D89="Know Well", 1, IF(D89="Know a Little", 0.5, 0)))/3</f>
+        <v>0</v>
+      </c>
+      <c r="E86" s="19"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C87" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="D87" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C88" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D88" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C89" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D89" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B90" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C90" s="25"/>
+      <c r="D90" s="8">
+        <f>(IF(D91="Know Well", 1, IF(D91="Know a Little", 0.5, 0))+IF(D92="Know Well", 1, IF(D92="Know a Little", 0.5, 0))+IF(D93="Know Well", 1, IF(D93="Know a Little", 0.5, 0))+IF(D94="Know Well", 1, IF(D94="Know a Little", 0.5, 0))+IF(D95="Know Well", 1, IF(D95="Know a Little", 0.5, 0)))/5</f>
+        <v>0</v>
+      </c>
+      <c r="E90" s="19"/>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C91" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D91" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C92" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D92" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C93" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D93" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C94" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="D94" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C95" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="D95" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B96" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C96" s="25"/>
+      <c r="D96" s="8">
+        <f>(IF(D97="Know Well", 1, IF(D97="Know a Little", 0.5, 0))+IF(D98="Know Well", 1, IF(D98="Know a Little", 0.5, 0))+IF(D99="Know Well", 1, IF(D99="Know a Little", 0.5, 0)))/3</f>
+        <v>0</v>
+      </c>
+      <c r="E96" s="19"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C97" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D97" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C98" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="D98" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C99" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D99" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B100" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C100" s="25"/>
+      <c r="D100" s="8">
+        <f>(IF(D101="Know Well", 1, IF(D101="Know a Little", 0.5, 0))+IF(D102="Know Well", 1, IF(D102="Know a Little", 0.5, 0))+IF(D103="Know Well", 1, IF(D103="Know a Little", 0.5, 0))+IF(D104="Know Well", 1, IF(D104="Know a Little", 0.5, 0))+IF(D105="Know Well", 1, IF(D105="Know a Little", 0.5, 0)))/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C101" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D101" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C102" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D102" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C103" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D103" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C104" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="D104" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C105" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D105" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B106" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C106" s="25"/>
+      <c r="D106" s="8">
+        <f>(IF(D107="Know Well", 1, IF(D107="Know a Little", 0.5, 0))+IF(D108="Know Well", 1, IF(D108="Know a Little", 0.5, 0))+IF(D109="Know Well", 1, IF(D109="Know a Little", 0.5, 0)))/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C107" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D107" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C108" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="D108" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C109" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D109" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A110" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C110" s="24"/>
+      <c r="D110" s="11">
+        <f>SUM(D111:D122)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B111" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D51" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B52" s="7" t="s">
+      <c r="C111" s="25"/>
+      <c r="D111" s="8">
+        <f>(IF(D112="Know Well", 1, IF(D112="Know a Little", 0.5, 0))+IF(D113="Know Well", 1, IF(D113="Know a Little", 0.5, 0))+IF(D114="Know Well", 1, IF(D114="Know a Little", 0.5, 0))+IF(D115="Know Well", 1, IF(D115="Know a Little", 0.5, 0))+IF(D116="Know Well", 1, IF(D116="Know a Little", 0.5, 0)))/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C112" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="D52" s="8">
-        <f>(IF(D53="Know Well", 1, IF(D53="Know a Little", 0.5, 0))+IF(D54="Know Well", 1, IF(D54="Know a Little", 0.5, 0))+IF(D55="Know Well", 1, IF(D55="Know a Little", 0.5, 0))+IF(D56="Know Well", 1, IF(D56="Know a Little", 0.5, 0))+IF(D57="Know Well", 1, IF(D57="Know a Little", 0.5, 0))+IF(D58="Know Well", 1, IF(D58="Know a Little", 0.5, 0)))/6</f>
+      <c r="D112" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C113" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D113" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C114" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D114" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="C115" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D115" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C116" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="D116" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B117" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C117" s="25"/>
+      <c r="D117" s="8">
+        <f>(IF(D118="Know Well", 1, IF(D118="Know a Little", 0.5, 0))+IF(D119="Know Well", 1, IF(D119="Know a Little", 0.5, 0))+IF(D120="Know Well", 1, IF(D120="Know a Little", 0.5, 0))+IF(D121="Know Well", 1, IF(D121="Know a Little", 0.5, 0))+IF(D122="Know Well", 1, IF(D122="Know a Little", 0.5, 0)))/5</f>
         <v>0</v>
       </c>
-      <c r="E52" s="19"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
-        <v>101</v>
-      </c>
-      <c r="D53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
-        <v>44</v>
-      </c>
-      <c r="D54" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
-        <v>43</v>
-      </c>
-      <c r="D55" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C56" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
-        <v>102</v>
-      </c>
-      <c r="D57" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C58" t="s">
-        <v>45</v>
-      </c>
-      <c r="D58" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B59" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D59" s="8">
-        <f>(IF(D60="Know Well", 1, IF(D60="Know a Little", 0.5, 0))+IF(D61="Know Well", 1, IF(D61="Know a Little", 0.5, 0)))/2</f>
-        <v>0</v>
-      </c>
-      <c r="E59" s="19"/>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C60" t="s">
-        <v>103</v>
-      </c>
-      <c r="D60" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C61" t="s">
-        <v>104</v>
-      </c>
-      <c r="D61" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B62" s="7" t="s">
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C118" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D118" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C119" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="D119" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C120" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D120" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C121" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D121" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C122" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="D62" s="8">
-        <f>(IF(D63="Know Well", 1, IF(D63="Know a Little", 0.5, 0))+IF(D64="Know Well", 1, IF(D64="Know a Little", 0.5, 0)))/2</f>
-        <v>0</v>
-      </c>
-      <c r="E62" s="21"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
-        <v>107</v>
-      </c>
-      <c r="D63" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C64" t="s">
-        <v>108</v>
-      </c>
-      <c r="D64" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A65" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D65" s="11">
-        <f>SUM(D66:D95)/6</f>
-        <v>0</v>
-      </c>
-      <c r="E65" s="20"/>
-    </row>
-    <row r="66" spans="1:5" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B66" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D66" s="8">
-        <f>(IF(D67="Know Well", 1, IF(D67="Know a Little", 0.5, 0))+IF(D68="Know Well", 1, IF(D68="Know a Little", 0.5, 0)))/2</f>
-        <v>0</v>
-      </c>
-      <c r="E66" s="19"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C67" t="s">
-        <v>46</v>
-      </c>
-      <c r="D67" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C68" t="s">
-        <v>48</v>
-      </c>
-      <c r="D68" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B69" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D69" s="8">
-        <f>(IF(D70="Know Well", 1, IF(D70="Know a Little", 0.5, 0))+IF(D71="Know Well", 1, IF(D71="Know a Little", 0.5, 0))+IF(D72="Know Well", 1, IF(D72="Know a Little", 0.5, 0)))/3</f>
-        <v>0</v>
-      </c>
-      <c r="E69" s="19"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C70" t="s">
-        <v>143</v>
-      </c>
-      <c r="D70" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C71" t="s">
-        <v>50</v>
-      </c>
-      <c r="D71" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C72" t="s">
-        <v>109</v>
-      </c>
-      <c r="D72" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B73" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D73" s="8">
-        <f>(IF(D74="Know Well", 1, IF(D74="Know a Little", 0.5, 0))+IF(D75="Know Well", 1, IF(D75="Know a Little", 0.5, 0))+IF(D76="Know Well", 1, IF(D76="Know a Little", 0.5, 0))+IF(D77="Know Well", 1, IF(D77="Know a Little", 0.5, 0))+IF(D78="Know Well", 1, IF(D78="Know a Little", 0.5, 0)))/5</f>
-        <v>0</v>
-      </c>
-      <c r="E73" s="19"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C74" t="s">
-        <v>51</v>
-      </c>
-      <c r="D74" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C75" t="s">
-        <v>52</v>
-      </c>
-      <c r="D75" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C76" t="s">
-        <v>53</v>
-      </c>
-      <c r="D76" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C77" t="s">
-        <v>111</v>
-      </c>
-      <c r="D77" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C78" t="s">
-        <v>112</v>
-      </c>
-      <c r="D78" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B79" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D79" s="8">
-        <f>(IF(D80="Know Well", 1, IF(D80="Know a Little", 0.5, 0))+IF(D81="Know Well", 1, IF(D81="Know a Little", 0.5, 0))+IF(D82="Know Well", 1, IF(D82="Know a Little", 0.5, 0))+IF(D83="Know Well", 1, IF(D83="Know a Little", 0.5, 0))+IF(D84="Know Well", 1, IF(D84="Know a Little", 0.5, 0)))/5</f>
-        <v>0</v>
-      </c>
-      <c r="E79" s="19"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C80" t="s">
-        <v>114</v>
-      </c>
-      <c r="D80" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C81" t="s">
-        <v>115</v>
-      </c>
-      <c r="D81" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C82" t="s">
-        <v>116</v>
-      </c>
-      <c r="D82" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C83" t="s">
-        <v>117</v>
-      </c>
-      <c r="D83" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C84" t="s">
-        <v>118</v>
-      </c>
-      <c r="D84" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B85" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D85" s="8">
-        <f>(IF(D86="Know Well", 1, IF(D86="Know a Little", 0.5, 0))+IF(D87="Know Well", 1, IF(D87="Know a Little", 0.5, 0))+IF(D88="Know Well", 1, IF(D88="Know a Little", 0.5, 0))+IF(D89="Know Well", 1, IF(D89="Know a Little", 0.5, 0))+IF(D90="Know Well", 1, IF(D90="Know a Little", 0.5, 0)))/5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C86" t="s">
-        <v>119</v>
-      </c>
-      <c r="D86" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C87" t="s">
-        <v>120</v>
-      </c>
-      <c r="D87" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C88" t="s">
-        <v>121</v>
-      </c>
-      <c r="D88" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C89" t="s">
-        <v>122</v>
-      </c>
-      <c r="D89" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C90" t="s">
-        <v>123</v>
-      </c>
-      <c r="D90" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B91" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D91" s="8">
-        <f>(IF(D92="Know Well", 1, IF(D92="Know a Little", 0.5, 0))+IF(D93="Know Well", 1, IF(D93="Know a Little", 0.5, 0))+IF(D94="Know Well", 1, IF(D94="Know a Little", 0.5, 0))+IF(D95="Know Well", 1, IF(D95="Know a Little", 0.5, 0)))/4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C92" t="s">
-        <v>125</v>
-      </c>
-      <c r="D92" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C93" t="s">
-        <v>126</v>
-      </c>
-      <c r="D93" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C94" t="s">
-        <v>127</v>
-      </c>
-      <c r="D94" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C95" t="s">
-        <v>128</v>
-      </c>
-      <c r="D95" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A96" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D96" s="11">
-        <f>SUM(D97:D108)/2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B97" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D97" s="8">
-        <f>(IF(D98="Know Well", 1, IF(D98="Know a Little", 0.5, 0))+IF(D99="Know Well", 1, IF(D99="Know a Little", 0.5, 0))+IF(D100="Know Well", 1, IF(D100="Know a Little", 0.5, 0))+IF(D101="Know Well", 1, IF(D101="Know a Little", 0.5, 0))+IF(D102="Know Well", 1, IF(D102="Know a Little", 0.5, 0)))/5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C98" t="s">
-        <v>130</v>
-      </c>
-      <c r="D98" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C99" t="s">
-        <v>131</v>
-      </c>
-      <c r="D99" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C100" t="s">
-        <v>132</v>
-      </c>
-      <c r="D100" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C101" t="s">
-        <v>133</v>
-      </c>
-      <c r="D101" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C102" t="s">
-        <v>134</v>
-      </c>
-      <c r="D102" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B103" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D103" s="8">
-        <f>(IF(D104="Know Well", 1, IF(D104="Know a Little", 0.5, 0))+IF(D105="Know Well", 1, IF(D105="Know a Little", 0.5, 0))+IF(D106="Know Well", 1, IF(D106="Know a Little", 0.5, 0))+IF(D107="Know Well", 1, IF(D107="Know a Little", 0.5, 0))+IF(D108="Know Well", 1, IF(D108="Know a Little", 0.5, 0)))/5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C104" t="s">
-        <v>34</v>
-      </c>
-      <c r="D104" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C105" t="s">
-        <v>136</v>
-      </c>
-      <c r="D105" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C106" t="s">
-        <v>137</v>
-      </c>
-      <c r="D106" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C107" t="s">
-        <v>35</v>
-      </c>
-      <c r="D107" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C108" t="s">
-        <v>138</v>
-      </c>
-      <c r="D108" t="s">
+      <c r="D122" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D4:D10">
-    <cfRule type="cellIs" dxfId="128" priority="276" operator="equal">
+  <conditionalFormatting sqref="D4:D11 D36 D26:D31 D107:D109 D97:D99">
+    <cfRule type="cellIs" dxfId="116" priority="276" operator="equal">
       <formula>"No Idea"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D10">
-    <cfRule type="cellIs" dxfId="127" priority="275" operator="equal">
+  <conditionalFormatting sqref="D4:D11 D36 D26:D31 D107:D109 D97:D99">
+    <cfRule type="cellIs" dxfId="115" priority="275" operator="equal">
       <formula>"Know a Little"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D10">
-    <cfRule type="cellIs" dxfId="126" priority="274" operator="equal">
+  <conditionalFormatting sqref="D4:D11 D36 D26:D31 D107:D109 D97:D99">
+    <cfRule type="cellIs" dxfId="114" priority="274" operator="equal">
       <formula>"Know Well"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="cellIs" dxfId="125" priority="174" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="174" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="cellIs" dxfId="124" priority="173" operator="lessThan">
+    <cfRule type="cellIs" dxfId="112" priority="173" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="cellIs" dxfId="123" priority="172" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="122" priority="186" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="121" priority="185" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="120" priority="184" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="119" priority="141" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="118" priority="140" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="117" priority="139" operator="between">
+    <cfRule type="cellIs" dxfId="111" priority="172" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="cellIs" dxfId="110" priority="186" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="cellIs" dxfId="109" priority="185" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="cellIs" dxfId="108" priority="184" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D117">
+    <cfRule type="cellIs" dxfId="107" priority="141" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D117">
+    <cfRule type="cellIs" dxfId="106" priority="140" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D117">
+    <cfRule type="cellIs" dxfId="105" priority="139" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="116" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="135" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="115" priority="134" operator="lessThan">
+    <cfRule type="cellIs" dxfId="103" priority="134" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="114" priority="133" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="113" priority="126" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="112" priority="125" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="111" priority="124" operator="between">
+    <cfRule type="cellIs" dxfId="102" priority="133" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D77">
+    <cfRule type="cellIs" dxfId="101" priority="126" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D77">
+    <cfRule type="cellIs" dxfId="100" priority="125" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D77">
+    <cfRule type="cellIs" dxfId="99" priority="124" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D110">
+    <cfRule type="cellIs" dxfId="98" priority="123" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D110">
+    <cfRule type="cellIs" dxfId="97" priority="122" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D110">
+    <cfRule type="cellIs" dxfId="96" priority="121" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:D15">
+    <cfRule type="cellIs" dxfId="95" priority="120" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:D15">
+    <cfRule type="cellIs" dxfId="94" priority="119" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:D15">
+    <cfRule type="cellIs" dxfId="93" priority="118" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17:D23">
+    <cfRule type="cellIs" dxfId="92" priority="117" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17:D23">
+    <cfRule type="cellIs" dxfId="91" priority="116" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17:D23">
+    <cfRule type="cellIs" dxfId="90" priority="115" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33:D38">
+    <cfRule type="cellIs" dxfId="89" priority="108" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33:D38">
+    <cfRule type="cellIs" dxfId="88" priority="107" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33:D38">
+    <cfRule type="cellIs" dxfId="87" priority="106" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40:D44">
+    <cfRule type="cellIs" dxfId="86" priority="105" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40:D44">
+    <cfRule type="cellIs" dxfId="85" priority="104" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40:D44">
+    <cfRule type="cellIs" dxfId="84" priority="103" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59:D60">
+    <cfRule type="cellIs" dxfId="83" priority="102" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59:D60">
+    <cfRule type="cellIs" dxfId="82" priority="101" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59:D60">
+    <cfRule type="cellIs" dxfId="81" priority="100" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47:D51">
+    <cfRule type="cellIs" dxfId="80" priority="99" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47:D51">
+    <cfRule type="cellIs" dxfId="79" priority="98" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47:D51">
+    <cfRule type="cellIs" dxfId="78" priority="97" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53:D60">
+    <cfRule type="cellIs" dxfId="77" priority="96" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53:D60">
+    <cfRule type="cellIs" dxfId="76" priority="95" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53:D60">
+    <cfRule type="cellIs" dxfId="75" priority="94" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62:D67">
+    <cfRule type="cellIs" dxfId="74" priority="93" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62:D67">
+    <cfRule type="cellIs" dxfId="73" priority="92" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62:D67">
+    <cfRule type="cellIs" dxfId="72" priority="91" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D106">
+    <cfRule type="cellIs" dxfId="71" priority="54" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D106">
+    <cfRule type="cellIs" dxfId="70" priority="53" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D106">
+    <cfRule type="cellIs" dxfId="69" priority="52" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D69:D76">
+    <cfRule type="cellIs" dxfId="68" priority="87" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D69:D76">
+    <cfRule type="cellIs" dxfId="67" priority="86" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D69:D76">
+    <cfRule type="cellIs" dxfId="66" priority="85" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D79:D85">
+    <cfRule type="cellIs" dxfId="65" priority="84" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D79:D85">
+    <cfRule type="cellIs" dxfId="64" priority="83" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D79:D85">
+    <cfRule type="cellIs" dxfId="63" priority="82" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D89">
+    <cfRule type="cellIs" dxfId="62" priority="81" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D89">
+    <cfRule type="cellIs" dxfId="61" priority="80" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D89">
+    <cfRule type="cellIs" dxfId="60" priority="79" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D91:D95">
+    <cfRule type="cellIs" dxfId="59" priority="78" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D91:D95">
+    <cfRule type="cellIs" dxfId="58" priority="77" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D91:D95">
+    <cfRule type="cellIs" dxfId="57" priority="76" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D101:D105">
+    <cfRule type="cellIs" dxfId="56" priority="72" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D101:D105">
+    <cfRule type="cellIs" dxfId="55" priority="71" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D101:D105">
+    <cfRule type="cellIs" dxfId="54" priority="70" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D112:D116">
+    <cfRule type="cellIs" dxfId="53" priority="66" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D112:D116">
+    <cfRule type="cellIs" dxfId="52" priority="65" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D112:D116">
+    <cfRule type="cellIs" dxfId="51" priority="64" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D118:D122">
+    <cfRule type="cellIs" dxfId="50" priority="63" operator="equal">
+      <formula>"No Idea"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D118:D122">
+    <cfRule type="cellIs" dxfId="49" priority="62" operator="equal">
+      <formula>"Know a Little"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D118:D122">
+    <cfRule type="cellIs" dxfId="48" priority="61" operator="equal">
+      <formula>"Know Well"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100">
+    <cfRule type="cellIs" dxfId="47" priority="51" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100">
+    <cfRule type="cellIs" dxfId="46" priority="50" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100">
+    <cfRule type="cellIs" dxfId="45" priority="49" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="44" priority="1" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D111">
+    <cfRule type="cellIs" dxfId="43" priority="57" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D111">
+    <cfRule type="cellIs" dxfId="42" priority="56" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D111">
+    <cfRule type="cellIs" dxfId="41" priority="55" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D96">
-    <cfRule type="cellIs" dxfId="110" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="48" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D96">
-    <cfRule type="cellIs" dxfId="109" priority="122" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="47" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D96">
-    <cfRule type="cellIs" dxfId="108" priority="121" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D15">
-    <cfRule type="cellIs" dxfId="107" priority="120" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D15">
-    <cfRule type="cellIs" dxfId="106" priority="119" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D15">
-    <cfRule type="cellIs" dxfId="105" priority="118" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D23">
-    <cfRule type="cellIs" dxfId="104" priority="117" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D23">
-    <cfRule type="cellIs" dxfId="103" priority="116" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D23">
-    <cfRule type="cellIs" dxfId="102" priority="115" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26:D31">
-    <cfRule type="cellIs" dxfId="101" priority="111" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26:D31">
-    <cfRule type="cellIs" dxfId="100" priority="110" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26:D31">
-    <cfRule type="cellIs" dxfId="99" priority="109" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33:D36">
-    <cfRule type="cellIs" dxfId="98" priority="108" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33:D36">
-    <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33:D36">
-    <cfRule type="cellIs" dxfId="96" priority="106" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D41">
-    <cfRule type="cellIs" dxfId="95" priority="105" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D41">
-    <cfRule type="cellIs" dxfId="94" priority="104" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D41">
-    <cfRule type="cellIs" dxfId="93" priority="103" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44:D45">
-    <cfRule type="cellIs" dxfId="92" priority="102" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44:D45">
-    <cfRule type="cellIs" dxfId="91" priority="101" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44:D45">
-    <cfRule type="cellIs" dxfId="90" priority="100" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47:D51">
-    <cfRule type="cellIs" dxfId="89" priority="99" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47:D51">
-    <cfRule type="cellIs" dxfId="88" priority="98" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47:D51">
-    <cfRule type="cellIs" dxfId="87" priority="97" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53:D58">
-    <cfRule type="cellIs" dxfId="86" priority="96" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53:D58">
-    <cfRule type="cellIs" dxfId="85" priority="95" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53:D58">
-    <cfRule type="cellIs" dxfId="84" priority="94" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60:D61">
-    <cfRule type="cellIs" dxfId="83" priority="93" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60:D61">
-    <cfRule type="cellIs" dxfId="82" priority="92" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60:D61">
-    <cfRule type="cellIs" dxfId="81" priority="91" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D91">
-    <cfRule type="cellIs" dxfId="80" priority="54" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D91">
-    <cfRule type="cellIs" dxfId="79" priority="53" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D91">
-    <cfRule type="cellIs" dxfId="78" priority="52" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63:D64">
-    <cfRule type="cellIs" dxfId="77" priority="87" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63:D64">
-    <cfRule type="cellIs" dxfId="76" priority="86" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63:D64">
-    <cfRule type="cellIs" dxfId="75" priority="85" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67:D68">
-    <cfRule type="cellIs" dxfId="74" priority="84" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67:D68">
-    <cfRule type="cellIs" dxfId="73" priority="83" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67:D68">
-    <cfRule type="cellIs" dxfId="72" priority="82" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D70:D72">
-    <cfRule type="cellIs" dxfId="71" priority="81" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D70:D72">
-    <cfRule type="cellIs" dxfId="70" priority="80" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D70:D72">
-    <cfRule type="cellIs" dxfId="69" priority="79" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D74:D78">
-    <cfRule type="cellIs" dxfId="68" priority="78" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D74:D78">
-    <cfRule type="cellIs" dxfId="67" priority="77" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D74:D78">
-    <cfRule type="cellIs" dxfId="66" priority="76" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D80:D84">
-    <cfRule type="cellIs" dxfId="65" priority="75" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D80:D84">
-    <cfRule type="cellIs" dxfId="64" priority="74" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D80:D84">
-    <cfRule type="cellIs" dxfId="63" priority="73" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D86:D90">
-    <cfRule type="cellIs" dxfId="62" priority="72" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D86:D90">
-    <cfRule type="cellIs" dxfId="61" priority="71" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D86:D90">
-    <cfRule type="cellIs" dxfId="60" priority="70" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D92:D95">
-    <cfRule type="cellIs" dxfId="59" priority="69" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D92:D95">
-    <cfRule type="cellIs" dxfId="58" priority="68" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D92:D95">
-    <cfRule type="cellIs" dxfId="57" priority="67" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D98:D102">
-    <cfRule type="cellIs" dxfId="56" priority="66" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D98:D102">
-    <cfRule type="cellIs" dxfId="55" priority="65" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D98:D102">
-    <cfRule type="cellIs" dxfId="54" priority="64" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D104:D108">
-    <cfRule type="cellIs" dxfId="53" priority="63" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D104:D108">
-    <cfRule type="cellIs" dxfId="52" priority="62" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D104:D108">
-    <cfRule type="cellIs" dxfId="51" priority="61" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="50" priority="51" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="49" priority="50" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="48" priority="49" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="47" priority="1" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D97">
-    <cfRule type="cellIs" dxfId="46" priority="57" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D97">
-    <cfRule type="cellIs" dxfId="45" priority="56" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D97">
-    <cfRule type="cellIs" dxfId="44" priority="55" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D79">
-    <cfRule type="cellIs" dxfId="43" priority="48" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D79">
-    <cfRule type="cellIs" dxfId="42" priority="47" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D79">
-    <cfRule type="cellIs" dxfId="41" priority="46" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="40" priority="45" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="39" priority="44" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="38" priority="43" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D69">
-    <cfRule type="cellIs" dxfId="37" priority="42" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D69">
-    <cfRule type="cellIs" dxfId="36" priority="41" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D69">
-    <cfRule type="cellIs" dxfId="35" priority="40" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
-    <cfRule type="cellIs" dxfId="34" priority="39" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
-    <cfRule type="cellIs" dxfId="33" priority="38" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
-    <cfRule type="cellIs" dxfId="32" priority="37" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="cellIs" dxfId="31" priority="36" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="cellIs" dxfId="30" priority="35" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="cellIs" dxfId="29" priority="34" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="cellIs" dxfId="28" priority="33" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="cellIs" dxfId="27" priority="32" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="cellIs" dxfId="26" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="38" priority="46" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D90">
+    <cfRule type="cellIs" dxfId="37" priority="45" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D90">
+    <cfRule type="cellIs" dxfId="36" priority="44" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D90">
+    <cfRule type="cellIs" dxfId="35" priority="43" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D86">
+    <cfRule type="cellIs" dxfId="34" priority="42" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D86">
+    <cfRule type="cellIs" dxfId="33" priority="41" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D86">
+    <cfRule type="cellIs" dxfId="32" priority="40" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D78">
+    <cfRule type="cellIs" dxfId="31" priority="39" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D78">
+    <cfRule type="cellIs" dxfId="30" priority="38" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D78">
+    <cfRule type="cellIs" dxfId="29" priority="37" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule type="cellIs" dxfId="28" priority="36" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule type="cellIs" dxfId="27" priority="35" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D68">
+    <cfRule type="cellIs" dxfId="26" priority="34" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="cellIs" dxfId="25" priority="33" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="cellIs" dxfId="24" priority="32" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="cellIs" dxfId="23" priority="31" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="cellIs" dxfId="25" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="30" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="cellIs" dxfId="24" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="29" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="cellIs" dxfId="23" priority="28" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="cellIs" dxfId="22" priority="27" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="cellIs" dxfId="21" priority="26" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="cellIs" dxfId="20" priority="25" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="20" priority="28" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
     <cfRule type="cellIs" dxfId="19" priority="24" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
+  <conditionalFormatting sqref="D12">
     <cfRule type="cellIs" dxfId="18" priority="23" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
+  <conditionalFormatting sqref="D12">
     <cfRule type="cellIs" dxfId="17" priority="22" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
+  <conditionalFormatting sqref="D45">
     <cfRule type="cellIs" dxfId="16" priority="21" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
+  <conditionalFormatting sqref="D45">
     <cfRule type="cellIs" dxfId="15" priority="20" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
+  <conditionalFormatting sqref="D45">
     <cfRule type="cellIs" dxfId="14" priority="19" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
@@ -4301,16 +4319,16 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>'Other Values'!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D4:D10 D12:D15 D17:D23 D26:D31 D33:D36 D38:D41 D44:D45 D47:D51 D53:D58 D60:D61 D63:D64 D67:D68 D70:D72 D74:D78 D80:D84 D86:D90 D92:D95 D98:D102 D104:D108</xm:sqref>
+          <xm:sqref>D118:D122 D13:D15 D17:D23 D33:D38 D47:D51 D53:D60 D40:D44 D97:D99 D107:D109 D87:D89 D91:D95 D101:D105 D112:D116 D4:D11 D26:D31 D62:D67 D79:D85 D69:D76</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4319,34 +4337,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>

</xml_diff>